<commit_message>
Updated .gitignore and added xlsx sheet for working examples
</commit_message>
<xml_diff>
--- a/01-intro-basics/data/varespec.xlsx
+++ b/01-intro-basics/data/varespec.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="varespec.csv" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Cal.vul</t>
   </si>
@@ -31,9 +31,6 @@
   </si>
   <si>
     <t>Vac.myr</t>
-  </si>
-  <si>
-    <t>Vac.vit</t>
   </si>
   <si>
     <t>Pin.syl</t>
@@ -181,10 +178,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -207,13 +220,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="11">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -546,14 +579,14 @@
   <dimension ref="A1:AU28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:47">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -568,127 +601,127 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>30</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>31</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" t="s">
-        <v>42</v>
-      </c>
       <c r="AU1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:47">
@@ -1513,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="AU7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:47">
@@ -2338,7 +2371,7 @@
         <v>0</v>
       </c>
       <c r="AU13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:47">
@@ -2626,7 +2659,7 @@
         <v>0.13</v>
       </c>
       <c r="D16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -3040,7 +3073,7 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19">
         <v>1.98</v>
@@ -3437,7 +3470,7 @@
         <v>0.25</v>
       </c>
       <c r="AU21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:47">
@@ -3990,11 +4023,12 @@
     </row>
     <row r="28" spans="1:47">
       <c r="K28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>